<commit_message>
Updates from last week
</commit_message>
<xml_diff>
--- a/Mohammed Gm.xlsx
+++ b/Mohammed Gm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smart1\Documents\GitHub\addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smart1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95CC5EBB-6323-484E-9552-72CA6676DE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE57115-A1D0-46EC-B21E-0C0AFE121A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F418FB7F-82F8-4F58-877E-B0BF7B0ED534}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>[36] Al Khobar Branch (138)</t>
   </si>
@@ -81,15 +81,12 @@
   <si>
     <t>الخبر</t>
   </si>
-  <si>
-    <t>missing</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,15 +138,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="DroidArabicKufiRegular"/>
     </font>
   </fonts>
   <fills count="4">
@@ -167,7 +158,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -277,7 +268,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -597,7 +587,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,10 +673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C458B20C-1B04-4155-925E-B59A9F984BC9}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -725,7 +715,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="8">
-        <f t="shared" ref="A4:A18" si="0">(A3+1)</f>
+        <f t="shared" ref="A4:A28" si="0">(A3+1)</f>
         <v>260001484</v>
       </c>
       <c r="B4" s="8">
@@ -889,7 +879,10 @@
       <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" ht="15.75">
-      <c r="A19" s="8"/>
+      <c r="A19" s="8">
+        <f t="shared" si="0"/>
+        <v>260001499</v>
+      </c>
       <c r="B19" s="8">
         <f t="shared" si="1"/>
         <v>300061991</v>
@@ -897,7 +890,10 @@
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" ht="15.75">
-      <c r="A20" s="8"/>
+      <c r="A20" s="8">
+        <f t="shared" si="0"/>
+        <v>260001500</v>
+      </c>
       <c r="B20" s="8">
         <f t="shared" si="1"/>
         <v>300061992</v>
@@ -905,7 +901,10 @@
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="15.75">
-      <c r="A21" s="8"/>
+      <c r="A21" s="8">
+        <f t="shared" si="0"/>
+        <v>260001501</v>
+      </c>
       <c r="B21" s="8">
         <f t="shared" si="1"/>
         <v>300061993</v>
@@ -913,7 +912,10 @@
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" ht="15.75">
-      <c r="A22" s="8"/>
+      <c r="A22" s="8">
+        <f t="shared" si="0"/>
+        <v>260001502</v>
+      </c>
       <c r="B22" s="8">
         <f t="shared" si="1"/>
         <v>300061994</v>
@@ -921,7 +923,10 @@
       <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" ht="15.75">
-      <c r="A23" s="8"/>
+      <c r="A23" s="8">
+        <f t="shared" si="0"/>
+        <v>260001503</v>
+      </c>
       <c r="B23" s="8">
         <f t="shared" si="1"/>
         <v>300061995</v>
@@ -929,7 +934,10 @@
       <c r="C23" s="8"/>
     </row>
     <row r="24" spans="1:3" ht="15.75">
-      <c r="A24" s="8"/>
+      <c r="A24" s="8">
+        <f t="shared" si="0"/>
+        <v>260001504</v>
+      </c>
       <c r="B24" s="8">
         <f t="shared" si="1"/>
         <v>300061996</v>
@@ -937,7 +945,10 @@
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" ht="15.75">
-      <c r="A25" s="8"/>
+      <c r="A25" s="8">
+        <f t="shared" si="0"/>
+        <v>260001505</v>
+      </c>
       <c r="B25" s="8">
         <f t="shared" si="1"/>
         <v>300061997</v>
@@ -945,7 +956,10 @@
       <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" ht="15.75">
-      <c r="A26" s="8"/>
+      <c r="A26" s="8">
+        <f t="shared" si="0"/>
+        <v>260001506</v>
+      </c>
       <c r="B26" s="8">
         <f t="shared" si="1"/>
         <v>300061998</v>
@@ -953,7 +967,10 @@
       <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" ht="15.75">
-      <c r="A27" s="8"/>
+      <c r="A27" s="8">
+        <f t="shared" si="0"/>
+        <v>260001507</v>
+      </c>
       <c r="B27" s="8">
         <f t="shared" si="1"/>
         <v>300061999</v>
@@ -961,7 +978,10 @@
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" ht="15.75">
-      <c r="A28" s="8"/>
+      <c r="A28" s="8">
+        <f t="shared" si="0"/>
+        <v>260001508</v>
+      </c>
       <c r="B28" s="8">
         <f t="shared" si="1"/>
         <v>300062000</v>
@@ -1228,7 +1248,7 @@
     </row>
     <row r="68" spans="2:2" ht="15.75">
       <c r="B68" s="8">
-        <f t="shared" ref="B68:B80" si="2">(B67+1)</f>
+        <f t="shared" ref="B68:B100" si="2">(B67+1)</f>
         <v>300062040</v>
       </c>
     </row>
@@ -1269,22 +1289,160 @@
       </c>
     </row>
     <row r="75" spans="2:2" ht="15.75">
-      <c r="B75" s="8"/>
+      <c r="B75" s="8">
+        <f t="shared" si="2"/>
+        <v>300062047</v>
+      </c>
     </row>
     <row r="76" spans="2:2" ht="15.75">
-      <c r="B76" s="8"/>
+      <c r="B76" s="8">
+        <f t="shared" si="2"/>
+        <v>300062048</v>
+      </c>
     </row>
     <row r="77" spans="2:2" ht="15.75">
-      <c r="B77" s="8"/>
+      <c r="B77" s="8">
+        <f t="shared" si="2"/>
+        <v>300062049</v>
+      </c>
     </row>
     <row r="78" spans="2:2" ht="15.75">
-      <c r="B78" s="8"/>
+      <c r="B78" s="8">
+        <f t="shared" si="2"/>
+        <v>300062050</v>
+      </c>
     </row>
     <row r="79" spans="2:2" ht="15.75">
-      <c r="B79" s="8"/>
+      <c r="B79" s="8">
+        <f t="shared" si="2"/>
+        <v>300062051</v>
+      </c>
     </row>
     <row r="80" spans="2:2" ht="15.75">
-      <c r="B80" s="8"/>
+      <c r="B80" s="8">
+        <f t="shared" si="2"/>
+        <v>300062052</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" ht="15.75">
+      <c r="B81" s="8">
+        <f t="shared" si="2"/>
+        <v>300062053</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="15.75">
+      <c r="B82" s="8">
+        <f t="shared" si="2"/>
+        <v>300062054</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" ht="15.75">
+      <c r="B83" s="8">
+        <f t="shared" si="2"/>
+        <v>300062055</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" ht="15.75">
+      <c r="B84" s="8">
+        <f t="shared" si="2"/>
+        <v>300062056</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" ht="15.75">
+      <c r="B85" s="8">
+        <f t="shared" si="2"/>
+        <v>300062057</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" ht="15.75">
+      <c r="B86" s="8">
+        <f t="shared" si="2"/>
+        <v>300062058</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" ht="15.75">
+      <c r="B87" s="8">
+        <f t="shared" si="2"/>
+        <v>300062059</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" ht="15.75">
+      <c r="B88" s="8">
+        <f t="shared" si="2"/>
+        <v>300062060</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="15.75">
+      <c r="B89" s="8">
+        <f t="shared" si="2"/>
+        <v>300062061</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" ht="15.75">
+      <c r="B90" s="8">
+        <f t="shared" si="2"/>
+        <v>300062062</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" ht="15.75">
+      <c r="B91" s="8">
+        <f t="shared" si="2"/>
+        <v>300062063</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" ht="15.75">
+      <c r="B92" s="8">
+        <f t="shared" si="2"/>
+        <v>300062064</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" ht="15.75">
+      <c r="B93" s="8">
+        <f t="shared" si="2"/>
+        <v>300062065</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" ht="15.75">
+      <c r="B94" s="8">
+        <f t="shared" si="2"/>
+        <v>300062066</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" ht="15.75">
+      <c r="B95" s="8">
+        <f t="shared" si="2"/>
+        <v>300062067</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" ht="15.75">
+      <c r="B96" s="8">
+        <f t="shared" si="2"/>
+        <v>300062068</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" ht="15.75">
+      <c r="B97" s="8">
+        <f t="shared" si="2"/>
+        <v>300062069</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" ht="15.75">
+      <c r="B98" s="8">
+        <f t="shared" si="2"/>
+        <v>300062070</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" ht="15.75">
+      <c r="B99" s="8">
+        <f t="shared" si="2"/>
+        <v>300062071</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" ht="15.75">
+      <c r="B100" s="8">
+        <f t="shared" si="2"/>
+        <v>300062072</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1293,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAF1FD5-29EE-421C-AA0A-0A80037E3444}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1312,7 +1470,7 @@
       <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="9">
@@ -1322,24 +1480,27 @@
         <v>926000278</v>
       </c>
       <c r="C2" s="9"/>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="9">
         <f>(A2+1)</f>
         <v>930009026</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="9">
+        <f>(B2+1)</f>
+        <v>926000279</v>
+      </c>
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9">
-        <f t="shared" ref="A4:A20" si="0">(A3+1)</f>
+        <f t="shared" ref="A4:A28" si="0">(A3+1)</f>
         <v>930009027</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9">
+        <f>(B3+1)</f>
+        <v>926000280</v>
+      </c>
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:7">
@@ -1439,9 +1600,57 @@
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="12">
+      <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>930009043</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="9">
+        <f t="shared" si="0"/>
+        <v>930009044</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="9">
+        <f t="shared" si="0"/>
+        <v>930009045</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="9">
+        <f t="shared" si="0"/>
+        <v>930009046</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="9">
+        <f t="shared" si="0"/>
+        <v>930009047</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="9">
+        <f t="shared" si="0"/>
+        <v>930009048</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="9">
+        <f t="shared" si="0"/>
+        <v>930009049</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="9">
+        <f t="shared" si="0"/>
+        <v>930009050</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="9">
+        <f t="shared" si="0"/>
+        <v>930009051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>